<commit_message>
Fixed bugs in shapefile (missing countries)
</commit_message>
<xml_diff>
--- a/Data/Input/AllLocations_DASCO.xlsx
+++ b/Data/Input/AllLocations_DASCO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="1172">
   <si>
     <t xml:space="preserve">locationID</t>
   </si>
@@ -2900,6 +2900,645 @@
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriatic Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aegean Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agulhas Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alboran Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleutian Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amsterdam-St Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amundsen/Bellingshausen Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andaman and Nicobar Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andaman Sea Coral Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angolan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctic Peninsula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arabian (Persian) Gulf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arafura Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Araucanian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arnhem Coast to Gulf of Carpenteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auckland Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azores Canaries Madeira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baffin Bay - Davis Strait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bahamian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baltic Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banda Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bassian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaufort Sea - continental coast and shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaufort-Amundsen-Viscount Melville-Queen Maud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bight of Sofala/Swamp Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismarck Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonaparte Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bounty and Antipodes Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campbell Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Howe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cargados Carajos/Tromelin Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carolinian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celtic Seas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central and Southern Great Barrier Reef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Kuroshio Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Peru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Somali Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channels and Fjords of Southern Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chatham Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiapas-Nicaragua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiloense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chukchi Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clipperton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocos-Keeling/Christmas Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coral Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cortezian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delagoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East African Coral Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Antarctic Dronning Maud Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Antarctic Enderby Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Antarctic Wilkes Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Caroline Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East China Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Greenland Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Siberian Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Bering Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Galapagos Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Philippines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exmouth to Broome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faroe Plateau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiji Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floridian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gilbert/Ellis Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Australian Bight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greater Antilles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guayaquil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guianan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Aden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Alaska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea South</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea Upwelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Maine/Bay of Fundy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Oman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Papua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of St. Lawrence - Eastern Scotian Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Tonkin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halmahera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heard and Macdonald Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Arctic Archipelago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houtman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hudson Complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humboldtian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ionian Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamchatka Shelf and Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kara Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kermadec Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lancaster Sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptev Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leeuwin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesser Sunda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levantine Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lord Howe and Norfolk Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macquarie Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magdalena Transition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malacca Strait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malvinas/Falklands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manning-Hawkesbury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mariana Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquesas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mascarene Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexican Tropical Pacific</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namaqua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicoya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ningaloo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North American Pacific Fijordland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North and East Barents Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North and East Iceland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Greenland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Patagonian Gulfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeast Sulawesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeastern Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeastern Honshu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeastern New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern and Central Red Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Bay of Bengal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Galapagos Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Grand Banks - Southern Labrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Gulf of Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Labrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Monsoon Current Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Norway and Finnmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oregon, Washington, Vancouver Coast and Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oyashio Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palawan/North Borneo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama Bight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patagonian Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peter the First Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phoenix/Tokelau/Northern Cook Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puget Trough/Georgia Basin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapa-Pitcairn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revillagigedos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de la Plata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio Grande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ross Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saharan Upwelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sahelian Upwelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samoa Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Pedro and Sao Paulo Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scotian Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea of Japan/East Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea of Okhotsk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shark Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snares Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Society Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solomon Archipelago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solomon Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South and West Iceland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Australian Gulfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South European Atlantic Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Georgia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South India and Sri Lanka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Kuroshio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Orkney Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Sandwich Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Shetland Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeast Madagascar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeast Papua New Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeastern Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern California Bight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Cook/Austral Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Grand Banks - South Newfoundland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Gulf of Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Red Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Vietnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southwestern Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Helena and Ascension Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulawesi Sea/Makassar Strait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunda Shelf/Java Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three Kings-North Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonga Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torres Strait Northern Great Barrier Reef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trindade and Martin Vaz Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tristan Gough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuamotus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunisian Plateau/Gulf of Sidra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tweed-Moreton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uruguay-Buenos Aires Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weddell Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Caroline Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Greenland Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western and Northern Madagascar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Arabian Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Bassian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Galapagos Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Mediterranean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Sumatra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow Sea</t>
   </si>
 </sst>
 </file>
@@ -3022,13 +3661,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K283"/>
+  <dimension ref="A1:K512"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A256" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E266" activeCellId="0" sqref="E266"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A493" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D512" activeCellId="0" sqref="D512"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.49"/>
@@ -3542,7 +4181,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>57</v>
@@ -3571,7 +4210,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>66</v>
@@ -3603,7 +4242,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>69</v>
@@ -3632,7 +4271,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>74</v>
@@ -3655,7 +4294,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>77</v>
@@ -3681,7 +4320,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>81</v>
@@ -3713,7 +4352,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>84</v>
@@ -3745,7 +4384,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>88</v>
@@ -3777,7 +4416,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>91</v>
@@ -3809,7 +4448,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>94</v>
@@ -3841,7 +4480,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>97</v>
@@ -3867,7 +4506,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>100</v>
@@ -3899,7 +4538,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>103</v>
@@ -3931,7 +4570,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>106</v>
@@ -3966,7 +4605,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>113</v>
@@ -3998,7 +4637,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>116</v>
@@ -4024,7 +4663,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>120</v>
@@ -4056,7 +4695,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>124</v>
@@ -4079,7 +4718,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>124</v>
@@ -4102,7 +4741,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>124</v>
@@ -4125,7 +4764,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>130</v>
@@ -4157,7 +4796,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>130</v>
@@ -4186,7 +4825,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>135</v>
@@ -4221,7 +4860,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>139</v>
@@ -4244,7 +4883,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>142</v>
@@ -4267,7 +4906,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>145</v>
@@ -4299,7 +4938,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>148</v>
@@ -4331,7 +4970,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>151</v>
@@ -4363,7 +5002,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>154</v>
@@ -4392,7 +5031,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>154</v>
@@ -4424,7 +5063,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>160</v>
@@ -4456,7 +5095,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>165</v>
@@ -4491,7 +5130,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>170</v>
@@ -4523,7 +5162,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>174</v>
@@ -4558,7 +5197,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>180</v>
@@ -4590,7 +5229,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>183</v>
@@ -4625,7 +5264,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>188</v>
@@ -4654,7 +5293,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>192</v>
@@ -4686,7 +5325,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>192</v>
@@ -4721,7 +5360,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>199</v>
@@ -4753,7 +5392,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>202</v>
@@ -4782,7 +5421,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>205</v>
@@ -4814,7 +5453,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>208</v>
@@ -4846,7 +5485,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>211</v>
@@ -4878,7 +5517,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>214</v>
@@ -4913,7 +5552,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>219</v>
@@ -4948,7 +5587,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>225</v>
@@ -4980,7 +5619,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>228</v>
@@ -5012,7 +5651,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>231</v>
@@ -5047,7 +5686,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>236</v>
@@ -5076,7 +5715,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>239</v>
@@ -5108,7 +5747,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>242</v>
@@ -5140,7 +5779,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>245</v>
@@ -5172,7 +5811,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>248</v>
@@ -5204,7 +5843,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>252</v>
@@ -5236,7 +5875,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>255</v>
@@ -5265,7 +5904,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>255</v>
@@ -5297,7 +5936,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>260</v>
@@ -5329,7 +5968,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>263</v>
@@ -5361,7 +6000,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>266</v>
@@ -5393,7 +6032,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>269</v>
@@ -5425,7 +6064,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>272</v>
@@ -5460,7 +6099,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>272</v>
@@ -5495,7 +6134,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>272</v>
@@ -5530,7 +6169,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>280</v>
@@ -5562,7 +6201,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>283</v>
@@ -5594,7 +6233,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>286</v>
@@ -5626,7 +6265,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>290</v>
@@ -5652,7 +6291,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>294</v>
@@ -5681,7 +6320,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>299</v>
@@ -5716,7 +6355,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>304</v>
@@ -5751,7 +6390,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>304</v>
@@ -5783,7 +6422,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>310</v>
@@ -5815,7 +6454,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>313</v>
@@ -5844,7 +6483,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>313</v>
@@ -5876,7 +6515,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>319</v>
@@ -5908,7 +6547,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>322</v>
@@ -5940,7 +6579,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>325</v>
@@ -5972,7 +6611,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>328</v>
@@ -5995,7 +6634,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>331</v>
@@ -6027,7 +6666,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>334</v>
@@ -6050,7 +6689,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>337</v>
@@ -6082,7 +6721,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>340</v>
@@ -6114,7 +6753,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>344</v>
@@ -6146,7 +6785,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>347</v>
@@ -6178,7 +6817,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>351</v>
@@ -6210,7 +6849,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>354</v>
@@ -6242,7 +6881,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>354</v>
@@ -6274,7 +6913,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>358</v>
@@ -6306,7 +6945,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>362</v>
@@ -6329,7 +6968,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>365</v>
@@ -6361,7 +7000,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>368</v>
@@ -6393,7 +7032,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>372</v>
@@ -6425,7 +7064,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>375</v>
@@ -6460,7 +7099,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>379</v>
@@ -6489,7 +7128,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>382</v>
@@ -6512,7 +7151,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B113" s="0" t="s">
         <v>385</v>
@@ -6544,7 +7183,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>388</v>
@@ -6573,7 +7212,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>391</v>
@@ -6605,7 +7244,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>394</v>
@@ -6640,7 +7279,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>398</v>
@@ -6672,7 +7311,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>401</v>
@@ -6704,7 +7343,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>404</v>
@@ -6727,7 +7366,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>407</v>
@@ -6756,7 +7395,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>407</v>
@@ -6788,7 +7427,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>412</v>
@@ -6817,7 +7456,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B123" s="0" t="s">
         <v>417</v>
@@ -6840,7 +7479,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>420</v>
@@ -6875,7 +7514,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B125" s="0" t="s">
         <v>426</v>
@@ -6904,7 +7543,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>429</v>
@@ -6936,7 +7575,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>429</v>
@@ -6971,7 +7610,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>429</v>
@@ -7006,7 +7645,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>437</v>
@@ -7029,7 +7668,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>440</v>
@@ -7061,7 +7700,7 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>443</v>
@@ -7084,7 +7723,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B132" s="0" t="s">
         <v>446</v>
@@ -7116,7 +7755,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="n">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B133" s="0" t="s">
         <v>446</v>
@@ -7148,7 +7787,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B134" s="0" t="s">
         <v>446</v>
@@ -7183,7 +7822,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="n">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B135" s="0" t="s">
         <v>452</v>
@@ -7215,7 +7854,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="n">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B136" s="0" t="s">
         <v>455</v>
@@ -7247,7 +7886,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B137" s="0" t="s">
         <v>458</v>
@@ -7270,7 +7909,7 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="n">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B138" s="0" t="s">
         <v>461</v>
@@ -7299,7 +7938,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="n">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B139" s="0" t="s">
         <v>464</v>
@@ -7334,7 +7973,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B140" s="0" t="s">
         <v>469</v>
@@ -7366,7 +8005,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B141" s="0" t="s">
         <v>473</v>
@@ -7401,7 +8040,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="n">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>479</v>
@@ -7436,7 +8075,7 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B143" s="0" t="s">
         <v>485</v>
@@ -7459,7 +8098,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B144" s="0" t="s">
         <v>488</v>
@@ -7494,7 +8133,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B145" s="0" t="s">
         <v>492</v>
@@ -7517,7 +8156,7 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B146" s="0" t="s">
         <v>495</v>
@@ -7552,7 +8191,7 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B147" s="0" t="s">
         <v>500</v>
@@ -7575,7 +8214,7 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B148" s="0" t="s">
         <v>503</v>
@@ -7610,7 +8249,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B149" s="0" t="s">
         <v>507</v>
@@ -7642,7 +8281,7 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B150" s="0" t="s">
         <v>510</v>
@@ -7674,7 +8313,7 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B151" s="0" t="s">
         <v>513</v>
@@ -7706,7 +8345,7 @@
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B152" s="0" t="s">
         <v>516</v>
@@ -7738,7 +8377,7 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B153" s="0" t="s">
         <v>519</v>
@@ -7770,7 +8409,7 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B154" s="0" t="s">
         <v>522</v>
@@ -7802,7 +8441,7 @@
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="n">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B155" s="0" t="s">
         <v>525</v>
@@ -7834,7 +8473,7 @@
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B156" s="0" t="s">
         <v>528</v>
@@ -7866,7 +8505,7 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B157" s="0" t="s">
         <v>532</v>
@@ -7898,7 +8537,7 @@
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B158" s="0" t="s">
         <v>535</v>
@@ -7921,7 +8560,7 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B159" s="0" t="s">
         <v>538</v>
@@ -7956,7 +8595,7 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B160" s="0" t="s">
         <v>545</v>
@@ -7979,7 +8618,7 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B161" s="0" t="s">
         <v>548</v>
@@ -8011,7 +8650,7 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B162" s="0" t="s">
         <v>553</v>
@@ -8043,7 +8682,7 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B163" s="0" t="s">
         <v>556</v>
@@ -8072,7 +8711,7 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="n">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B164" s="0" t="s">
         <v>560</v>
@@ -8107,7 +8746,7 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B165" s="0" t="s">
         <v>566</v>
@@ -8139,7 +8778,7 @@
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="B166" s="0" t="s">
         <v>569</v>
@@ -8168,7 +8807,7 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B167" s="0" t="s">
         <v>573</v>
@@ -8200,7 +8839,7 @@
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B168" s="0" t="s">
         <v>576</v>
@@ -8232,7 +8871,7 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B169" s="0" t="s">
         <v>580</v>
@@ -8261,7 +8900,7 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B170" s="0" t="s">
         <v>584</v>
@@ -8293,7 +8932,7 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B171" s="0" t="s">
         <v>587</v>
@@ -8325,7 +8964,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B172" s="0" t="s">
         <v>590</v>
@@ -8357,7 +8996,7 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B173" s="0" t="s">
         <v>593</v>
@@ -8389,7 +9028,7 @@
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B174" s="0" t="s">
         <v>596</v>
@@ -8418,7 +9057,7 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B175" s="0" t="s">
         <v>596</v>
@@ -8447,7 +9086,7 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B176" s="0" t="s">
         <v>600</v>
@@ -8482,7 +9121,7 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="B177" s="0" t="s">
         <v>604</v>
@@ -8514,7 +9153,7 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B178" s="0" t="s">
         <v>607</v>
@@ -8543,7 +9182,7 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="n">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B179" s="0" t="s">
         <v>607</v>
@@ -8575,7 +9214,7 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="B180" s="0" t="s">
         <v>612</v>
@@ -8604,7 +9243,7 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="B181" s="0" t="s">
         <v>615</v>
@@ -8633,7 +9272,7 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="B182" s="0" t="s">
         <v>618</v>
@@ -8665,7 +9304,7 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="B183" s="0" t="s">
         <v>621</v>
@@ -8697,7 +9336,7 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="B184" s="0" t="s">
         <v>624</v>
@@ -8729,7 +9368,7 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B185" s="0" t="s">
         <v>628</v>
@@ -8764,7 +9403,7 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="n">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="B186" s="0" t="s">
         <v>632</v>
@@ -8796,7 +9435,7 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="B187" s="0" t="s">
         <v>635</v>
@@ -8828,7 +9467,7 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B188" s="0" t="s">
         <v>638</v>
@@ -8860,7 +9499,7 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B189" s="0" t="s">
         <v>642</v>
@@ -8892,7 +9531,7 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="B190" s="0" t="s">
         <v>646</v>
@@ -8924,7 +9563,7 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="B191" s="0" t="s">
         <v>649</v>
@@ -8956,7 +9595,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="n">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="B192" s="0" t="s">
         <v>652</v>
@@ -8982,7 +9621,7 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="n">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="B193" s="0" t="s">
         <v>655</v>
@@ -9017,7 +9656,7 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="n">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B194" s="0" t="s">
         <v>655</v>
@@ -9049,7 +9688,7 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="n">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="B195" s="0" t="s">
         <v>660</v>
@@ -9081,7 +9720,7 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="n">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B196" s="0" t="s">
         <v>663</v>
@@ -9113,7 +9752,7 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="n">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="B197" s="0" t="s">
         <v>666</v>
@@ -9145,7 +9784,7 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="n">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="B198" s="0" t="s">
         <v>669</v>
@@ -9177,7 +9816,7 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="n">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="B199" s="0" t="s">
         <v>673</v>
@@ -9209,7 +9848,7 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="n">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="B200" s="0" t="s">
         <v>676</v>
@@ -9241,7 +9880,7 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="n">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B201" s="0" t="s">
         <v>680</v>
@@ -9264,7 +9903,7 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="n">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="B202" s="0" t="s">
         <v>683</v>
@@ -9296,7 +9935,7 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="n">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="B203" s="0" t="s">
         <v>686</v>
@@ -9331,7 +9970,7 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="n">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B204" s="0" t="s">
         <v>690</v>
@@ -9363,7 +10002,7 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="n">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="B205" s="0" t="s">
         <v>694</v>
@@ -9395,7 +10034,7 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="n">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="B206" s="0" t="s">
         <v>697</v>
@@ -9424,7 +10063,7 @@
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="n">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="B207" s="0" t="s">
         <v>702</v>
@@ -9456,7 +10095,7 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="n">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="B208" s="0" t="s">
         <v>702</v>
@@ -9491,7 +10130,7 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="n">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B209" s="0" t="s">
         <v>702</v>
@@ -9526,7 +10165,7 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="n">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B210" s="0" t="s">
         <v>710</v>
@@ -9549,7 +10188,7 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="n">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B211" s="0" t="s">
         <v>713</v>
@@ -9581,7 +10220,7 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="n">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="B212" s="0" t="s">
         <v>716</v>
@@ -9613,7 +10252,7 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="n">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="B213" s="0" t="s">
         <v>719</v>
@@ -9648,7 +10287,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="n">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="B214" s="0" t="s">
         <v>724</v>
@@ -9680,7 +10319,7 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="n">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="B215" s="0" t="s">
         <v>727</v>
@@ -9703,7 +10342,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="n">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="B216" s="0" t="s">
         <v>731</v>
@@ -9735,7 +10374,7 @@
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="n">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B217" s="0" t="s">
         <v>736</v>
@@ -9767,7 +10406,7 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="n">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="B218" s="0" t="s">
         <v>739</v>
@@ -9799,7 +10438,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="n">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B219" s="0" t="s">
         <v>742</v>
@@ -9822,7 +10461,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="n">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="B220" s="0" t="s">
         <v>745</v>
@@ -9854,7 +10493,7 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="n">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="B221" s="0" t="s">
         <v>749</v>
@@ -9889,7 +10528,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="n">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="B222" s="0" t="s">
         <v>755</v>
@@ -9921,7 +10560,7 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="n">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B223" s="0" t="s">
         <v>758</v>
@@ -9953,7 +10592,7 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="n">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="B224" s="0" t="s">
         <v>761</v>
@@ -9985,7 +10624,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="n">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="B225" s="0" t="s">
         <v>761</v>
@@ -10014,7 +10653,7 @@
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="n">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="B226" s="0" t="s">
         <v>761</v>
@@ -10043,7 +10682,7 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="n">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B227" s="0" t="s">
         <v>768</v>
@@ -10075,7 +10714,7 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="n">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B228" s="0" t="s">
         <v>771</v>
@@ -10107,7 +10746,7 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="n">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="B229" s="0" t="s">
         <v>775</v>
@@ -10139,7 +10778,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="n">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="B230" s="0" t="s">
         <v>778</v>
@@ -10171,7 +10810,7 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="n">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="B231" s="0" t="s">
         <v>781</v>
@@ -10194,7 +10833,7 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="n">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="B232" s="0" t="s">
         <v>784</v>
@@ -10226,7 +10865,7 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="n">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="B233" s="0" t="s">
         <v>786</v>
@@ -10258,7 +10897,7 @@
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="n">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="B234" s="0" t="s">
         <v>789</v>
@@ -10290,7 +10929,7 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="n">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="B235" s="0" t="s">
         <v>792</v>
@@ -10325,7 +10964,7 @@
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="n">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B236" s="0" t="s">
         <v>796</v>
@@ -10348,7 +10987,7 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="n">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="B237" s="0" t="s">
         <v>219</v>
@@ -10380,7 +11019,7 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="n">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B238" s="0" t="s">
         <v>802</v>
@@ -10409,7 +11048,7 @@
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="n">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="B239" s="0" t="s">
         <v>806</v>
@@ -10444,7 +11083,7 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="n">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="B240" s="0" t="s">
         <v>810</v>
@@ -10473,7 +11112,7 @@
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="n">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B241" s="0" t="s">
         <v>814</v>
@@ -10505,7 +11144,7 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="n">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="B242" s="0" t="s">
         <v>817</v>
@@ -10537,7 +11176,7 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="n">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="B243" s="0" t="s">
         <v>817</v>
@@ -10569,7 +11208,7 @@
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="n">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="B244" s="0" t="s">
         <v>817</v>
@@ -10601,7 +11240,7 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="n">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="B245" s="0" t="s">
         <v>817</v>
@@ -10633,7 +11272,7 @@
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="n">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="B246" s="0" t="s">
         <v>817</v>
@@ -10665,7 +11304,7 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="n">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B247" s="0" t="s">
         <v>831</v>
@@ -10697,7 +11336,7 @@
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="n">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B248" s="0" t="s">
         <v>834</v>
@@ -10729,7 +11368,7 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="n">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="B249" s="0" t="s">
         <v>837</v>
@@ -10761,7 +11400,7 @@
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="n">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="B250" s="0" t="s">
         <v>841</v>
@@ -10784,7 +11423,7 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="n">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="B251" s="0" t="s">
         <v>844</v>
@@ -10810,7 +11449,7 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="n">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="B252" s="0" t="s">
         <v>849</v>
@@ -10833,7 +11472,7 @@
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="n">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="B253" s="0" t="s">
         <v>852</v>
@@ -10865,7 +11504,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="n">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="B254" s="0" t="s">
         <v>855</v>
@@ -10897,7 +11536,7 @@
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="n">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="B255" s="0" t="s">
         <v>858</v>
@@ -10929,7 +11568,7 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="n">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="B256" s="0" t="s">
         <v>844</v>
@@ -10952,7 +11591,7 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="n">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="B257" s="0" t="s">
         <v>864</v>
@@ -10975,7 +11614,7 @@
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="n">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="B258" s="0" t="s">
         <v>867</v>
@@ -11010,7 +11649,7 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="n">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="B259" s="0" t="s">
         <v>872</v>
@@ -11042,7 +11681,7 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="n">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="B260" s="0" t="s">
         <v>872</v>
@@ -11077,7 +11716,7 @@
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="n">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="B261" s="0" t="s">
         <v>878</v>
@@ -11109,7 +11748,7 @@
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="n">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="B262" s="0" t="s">
         <v>881</v>
@@ -11141,7 +11780,7 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="n">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="B263" s="0" t="s">
         <v>884</v>
@@ -11173,7 +11812,7 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="n">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="B264" s="0" t="s">
         <v>889</v>
@@ -11205,7 +11844,7 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="n">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="B265" s="0" t="s">
         <v>889</v>
@@ -11237,7 +11876,7 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="n">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="B266" s="0" t="s">
         <v>889</v>
@@ -11269,7 +11908,7 @@
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="n">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="B267" s="0" t="s">
         <v>898</v>
@@ -11301,7 +11940,7 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="n">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="B268" s="0" t="s">
         <v>901</v>
@@ -11324,7 +11963,7 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="n">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="B269" s="0" t="s">
         <v>904</v>
@@ -11350,7 +11989,7 @@
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="n">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="B270" s="0" t="s">
         <v>909</v>
@@ -11382,7 +12021,7 @@
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="n">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="B271" s="0" t="s">
         <v>913</v>
@@ -11417,7 +12056,7 @@
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="n">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="B272" s="0" t="s">
         <v>918</v>
@@ -11446,7 +12085,7 @@
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="n">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="B273" s="0" t="s">
         <v>922</v>
@@ -11481,7 +12120,7 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="n">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="B274" s="0" t="s">
         <v>928</v>
@@ -11507,7 +12146,7 @@
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="n">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="B275" s="0" t="s">
         <v>932</v>
@@ -11530,7 +12169,7 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="n">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="B276" s="0" t="s">
         <v>935</v>
@@ -11553,7 +12192,7 @@
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="n">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="B277" s="0" t="s">
         <v>938</v>
@@ -11582,7 +12221,7 @@
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="n">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="B278" s="0" t="s">
         <v>941</v>
@@ -11617,7 +12256,7 @@
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="n">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="B279" s="0" t="s">
         <v>941</v>
@@ -11649,7 +12288,7 @@
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="n">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="B280" s="0" t="s">
         <v>946</v>
@@ -11681,7 +12320,7 @@
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="n">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="B281" s="0" t="s">
         <v>949</v>
@@ -11713,7 +12352,7 @@
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="n">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="B282" s="0" t="s">
         <v>953</v>
@@ -11742,7 +12381,7 @@
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="n">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="B283" s="0" t="s">
         <v>956</v>
@@ -11767,6 +12406,1838 @@
       </c>
       <c r="K283" s="0" t="s">
         <v>958</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="n">
+        <v>283</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="n">
+        <v>284</v>
+      </c>
+      <c r="D285" s="0" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="n">
+        <v>285</v>
+      </c>
+      <c r="D286" s="0" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="n">
+        <v>286</v>
+      </c>
+      <c r="D287" s="0" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="D288" s="0" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="D289" s="0" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="n">
+        <v>289</v>
+      </c>
+      <c r="D290" s="0" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="D291" s="0" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="D292" s="0" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="n">
+        <v>292</v>
+      </c>
+      <c r="D293" s="0" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="n">
+        <v>293</v>
+      </c>
+      <c r="D294" s="0" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D295" s="0" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="0" t="n">
+        <v>295</v>
+      </c>
+      <c r="D296" s="0" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="n">
+        <v>296</v>
+      </c>
+      <c r="D297" s="0" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="n">
+        <v>297</v>
+      </c>
+      <c r="D298" s="0" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="n">
+        <v>298</v>
+      </c>
+      <c r="D299" s="0" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="0" t="n">
+        <v>299</v>
+      </c>
+      <c r="D300" s="0" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="D301" s="0" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="n">
+        <v>301</v>
+      </c>
+      <c r="D302" s="0" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="n">
+        <v>302</v>
+      </c>
+      <c r="D303" s="0" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="n">
+        <v>303</v>
+      </c>
+      <c r="D304" s="0" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="n">
+        <v>304</v>
+      </c>
+      <c r="D305" s="0" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="n">
+        <v>305</v>
+      </c>
+      <c r="D306" s="0" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="n">
+        <v>306</v>
+      </c>
+      <c r="D307" s="0" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="D308" s="0" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="D309" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="n">
+        <v>309</v>
+      </c>
+      <c r="D310" s="0" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="D311" s="0" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="n">
+        <v>311</v>
+      </c>
+      <c r="D312" s="0" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="D313" s="0" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="n">
+        <v>313</v>
+      </c>
+      <c r="D314" s="0" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="n">
+        <v>314</v>
+      </c>
+      <c r="D315" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="D316" s="0" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="D317" s="0" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="n">
+        <v>317</v>
+      </c>
+      <c r="D318" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D319" s="0" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="D320" s="0" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="D321" s="0" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="n">
+        <v>321</v>
+      </c>
+      <c r="D322" s="0" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="D323" s="0" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="n">
+        <v>323</v>
+      </c>
+      <c r="D324" s="0" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="n">
+        <v>324</v>
+      </c>
+      <c r="D325" s="0" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="D326" s="0" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="n">
+        <v>326</v>
+      </c>
+      <c r="D327" s="0" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="n">
+        <v>327</v>
+      </c>
+      <c r="D328" s="0" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="n">
+        <v>328</v>
+      </c>
+      <c r="D329" s="0" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="n">
+        <v>329</v>
+      </c>
+      <c r="D330" s="0" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="D331" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="n">
+        <v>331</v>
+      </c>
+      <c r="D332" s="0" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="n">
+        <v>332</v>
+      </c>
+      <c r="D333" s="0" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="n">
+        <v>333</v>
+      </c>
+      <c r="D334" s="0" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="n">
+        <v>334</v>
+      </c>
+      <c r="D335" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="D336" s="0" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="D337" s="0" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="D338" s="0" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="D339" s="0" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="n">
+        <v>339</v>
+      </c>
+      <c r="D340" s="0" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="n">
+        <v>340</v>
+      </c>
+      <c r="D341" s="0" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="n">
+        <v>341</v>
+      </c>
+      <c r="D342" s="0" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D343" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="n">
+        <v>343</v>
+      </c>
+      <c r="D344" s="0" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="D345" s="0" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="n">
+        <v>345</v>
+      </c>
+      <c r="D346" s="0" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="n">
+        <v>346</v>
+      </c>
+      <c r="D347" s="0" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="n">
+        <v>347</v>
+      </c>
+      <c r="D348" s="0" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="n">
+        <v>348</v>
+      </c>
+      <c r="D349" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="n">
+        <v>349</v>
+      </c>
+      <c r="D350" s="0" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="D351" s="0" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="D352" s="0" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="n">
+        <v>352</v>
+      </c>
+      <c r="D353" s="0" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="n">
+        <v>353</v>
+      </c>
+      <c r="D354" s="0" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="n">
+        <v>354</v>
+      </c>
+      <c r="D355" s="0" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="n">
+        <v>355</v>
+      </c>
+      <c r="D356" s="0" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="n">
+        <v>356</v>
+      </c>
+      <c r="D357" s="0" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="n">
+        <v>357</v>
+      </c>
+      <c r="D358" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="n">
+        <v>358</v>
+      </c>
+      <c r="D359" s="0" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="n">
+        <v>359</v>
+      </c>
+      <c r="D360" s="0" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="D361" s="0" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="n">
+        <v>361</v>
+      </c>
+      <c r="D362" s="0" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="n">
+        <v>362</v>
+      </c>
+      <c r="D363" s="0" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="n">
+        <v>363</v>
+      </c>
+      <c r="D364" s="0" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="n">
+        <v>364</v>
+      </c>
+      <c r="D365" s="0" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="D366" s="0" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="D367" s="0" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="n">
+        <v>367</v>
+      </c>
+      <c r="D368" s="0" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="n">
+        <v>368</v>
+      </c>
+      <c r="D369" s="0" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="n">
+        <v>369</v>
+      </c>
+      <c r="D370" s="0" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="n">
+        <v>370</v>
+      </c>
+      <c r="D371" s="0" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="n">
+        <v>371</v>
+      </c>
+      <c r="D372" s="0" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="0" t="n">
+        <v>372</v>
+      </c>
+      <c r="D373" s="0" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="n">
+        <v>373</v>
+      </c>
+      <c r="D374" s="0" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="0" t="n">
+        <v>374</v>
+      </c>
+      <c r="D375" s="0" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="n">
+        <v>375</v>
+      </c>
+      <c r="D376" s="0" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="0" t="n">
+        <v>376</v>
+      </c>
+      <c r="D377" s="0" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="0" t="n">
+        <v>377</v>
+      </c>
+      <c r="D378" s="0" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="n">
+        <v>378</v>
+      </c>
+      <c r="D379" s="0" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="0" t="n">
+        <v>379</v>
+      </c>
+      <c r="D380" s="0" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="D381" s="0" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="0" t="n">
+        <v>381</v>
+      </c>
+      <c r="D382" s="0" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="0" t="n">
+        <v>382</v>
+      </c>
+      <c r="D383" s="0" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="0" t="n">
+        <v>383</v>
+      </c>
+      <c r="D384" s="0" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="0" t="n">
+        <v>384</v>
+      </c>
+      <c r="D385" s="0" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="0" t="n">
+        <v>385</v>
+      </c>
+      <c r="D386" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="0" t="n">
+        <v>386</v>
+      </c>
+      <c r="D387" s="0" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="0" t="n">
+        <v>387</v>
+      </c>
+      <c r="D388" s="0" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="0" t="n">
+        <v>388</v>
+      </c>
+      <c r="D389" s="0" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="0" t="n">
+        <v>389</v>
+      </c>
+      <c r="D390" s="0" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="D391" s="0" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="0" t="n">
+        <v>391</v>
+      </c>
+      <c r="D392" s="0" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="0" t="n">
+        <v>392</v>
+      </c>
+      <c r="D393" s="0" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A394" s="0" t="n">
+        <v>393</v>
+      </c>
+      <c r="D394" s="0" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A395" s="0" t="n">
+        <v>394</v>
+      </c>
+      <c r="D395" s="0" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="0" t="n">
+        <v>395</v>
+      </c>
+      <c r="D396" s="0" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="0" t="n">
+        <v>396</v>
+      </c>
+      <c r="D397" s="0" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A398" s="0" t="n">
+        <v>397</v>
+      </c>
+      <c r="D398" s="0" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A399" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="D399" s="0" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="0" t="n">
+        <v>399</v>
+      </c>
+      <c r="D400" s="0" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A401" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="D401" s="0" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="0" t="n">
+        <v>401</v>
+      </c>
+      <c r="D402" s="0" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="0" t="n">
+        <v>402</v>
+      </c>
+      <c r="D403" s="0" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="0" t="n">
+        <v>403</v>
+      </c>
+      <c r="D404" s="0" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="0" t="n">
+        <v>404</v>
+      </c>
+      <c r="D405" s="0" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="0" t="n">
+        <v>405</v>
+      </c>
+      <c r="D406" s="0" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="0" t="n">
+        <v>406</v>
+      </c>
+      <c r="D407" s="0" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="0" t="n">
+        <v>407</v>
+      </c>
+      <c r="D408" s="0" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="0" t="n">
+        <v>408</v>
+      </c>
+      <c r="D409" s="0" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="0" t="n">
+        <v>409</v>
+      </c>
+      <c r="D410" s="0" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A411" s="0" t="n">
+        <v>410</v>
+      </c>
+      <c r="D411" s="0" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A412" s="0" t="n">
+        <v>411</v>
+      </c>
+      <c r="D412" s="0" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="0" t="n">
+        <v>412</v>
+      </c>
+      <c r="D413" s="0" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="0" t="n">
+        <v>413</v>
+      </c>
+      <c r="D414" s="0" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="0" t="n">
+        <v>414</v>
+      </c>
+      <c r="D415" s="0" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="0" t="n">
+        <v>415</v>
+      </c>
+      <c r="D416" s="0" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="0" t="n">
+        <v>416</v>
+      </c>
+      <c r="D417" s="0" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="0" t="n">
+        <v>417</v>
+      </c>
+      <c r="D418" s="0" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A419" s="0" t="n">
+        <v>418</v>
+      </c>
+      <c r="D419" s="0" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A420" s="0" t="n">
+        <v>419</v>
+      </c>
+      <c r="D420" s="0" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="0" t="n">
+        <v>420</v>
+      </c>
+      <c r="D421" s="0" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="0" t="n">
+        <v>421</v>
+      </c>
+      <c r="D422" s="0" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="D423" s="0" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A424" s="0" t="n">
+        <v>423</v>
+      </c>
+      <c r="D424" s="0" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="D425" s="0" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="D426" s="0" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="0" t="n">
+        <v>426</v>
+      </c>
+      <c r="D427" s="0" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="0" t="n">
+        <v>427</v>
+      </c>
+      <c r="D428" s="0" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="0" t="n">
+        <v>428</v>
+      </c>
+      <c r="D429" s="0" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="0" t="n">
+        <v>429</v>
+      </c>
+      <c r="D430" s="0" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="0" t="n">
+        <v>430</v>
+      </c>
+      <c r="D431" s="0" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="0" t="n">
+        <v>431</v>
+      </c>
+      <c r="D432" s="0" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="D433" s="0" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="D434" s="0" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="0" t="n">
+        <v>434</v>
+      </c>
+      <c r="D435" s="0" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A436" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="D436" s="0" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="0" t="n">
+        <v>436</v>
+      </c>
+      <c r="D437" s="0" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="0" t="n">
+        <v>437</v>
+      </c>
+      <c r="D438" s="0" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="0" t="n">
+        <v>438</v>
+      </c>
+      <c r="D439" s="0" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="0" t="n">
+        <v>439</v>
+      </c>
+      <c r="D440" s="0" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="0" t="n">
+        <v>440</v>
+      </c>
+      <c r="D441" s="0" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="0" t="n">
+        <v>441</v>
+      </c>
+      <c r="D442" s="0" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="D443" s="0" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A444" s="0" t="n">
+        <v>443</v>
+      </c>
+      <c r="D444" s="0" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="0" t="n">
+        <v>444</v>
+      </c>
+      <c r="D445" s="0" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A446" s="0" t="n">
+        <v>445</v>
+      </c>
+      <c r="D446" s="0" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="0" t="n">
+        <v>446</v>
+      </c>
+      <c r="D447" s="0" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A448" s="0" t="n">
+        <v>447</v>
+      </c>
+      <c r="D448" s="0" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="0" t="n">
+        <v>448</v>
+      </c>
+      <c r="D449" s="0" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A450" s="0" t="n">
+        <v>449</v>
+      </c>
+      <c r="D450" s="0" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A451" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="D451" s="0" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A452" s="0" t="n">
+        <v>451</v>
+      </c>
+      <c r="D452" s="0" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="0" t="n">
+        <v>452</v>
+      </c>
+      <c r="D453" s="0" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="0" t="n">
+        <v>453</v>
+      </c>
+      <c r="D454" s="0" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="D455" s="0" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="0" t="n">
+        <v>455</v>
+      </c>
+      <c r="D456" s="0" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A457" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="D457" s="0" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="0" t="n">
+        <v>457</v>
+      </c>
+      <c r="D458" s="0" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="0" t="n">
+        <v>458</v>
+      </c>
+      <c r="D459" s="0" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="0" t="n">
+        <v>459</v>
+      </c>
+      <c r="D460" s="0" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="D461" s="0" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="0" t="n">
+        <v>461</v>
+      </c>
+      <c r="D462" s="0" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="0" t="n">
+        <v>462</v>
+      </c>
+      <c r="D463" s="0" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="0" t="n">
+        <v>463</v>
+      </c>
+      <c r="D464" s="0" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="0" t="n">
+        <v>464</v>
+      </c>
+      <c r="D465" s="0" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A466" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="D466" s="0" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="0" t="n">
+        <v>466</v>
+      </c>
+      <c r="D467" s="0" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="0" t="n">
+        <v>467</v>
+      </c>
+      <c r="D468" s="0" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="0" t="n">
+        <v>468</v>
+      </c>
+      <c r="D469" s="0" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="0" t="n">
+        <v>469</v>
+      </c>
+      <c r="D470" s="0" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="0" t="n">
+        <v>470</v>
+      </c>
+      <c r="D471" s="0" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="0" t="n">
+        <v>471</v>
+      </c>
+      <c r="D472" s="0" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="0" t="n">
+        <v>472</v>
+      </c>
+      <c r="D473" s="0" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="0" t="n">
+        <v>473</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="0" t="n">
+        <v>474</v>
+      </c>
+      <c r="D475" s="0" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="0" t="n">
+        <v>475</v>
+      </c>
+      <c r="D476" s="0" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="0" t="n">
+        <v>476</v>
+      </c>
+      <c r="D477" s="0" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="0" t="n">
+        <v>477</v>
+      </c>
+      <c r="D478" s="0" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="0" t="n">
+        <v>478</v>
+      </c>
+      <c r="D479" s="0" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="0" t="n">
+        <v>479</v>
+      </c>
+      <c r="D480" s="0" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="0" t="n">
+        <v>480</v>
+      </c>
+      <c r="D481" s="0" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="0" t="n">
+        <v>481</v>
+      </c>
+      <c r="D482" s="0" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="0" t="n">
+        <v>482</v>
+      </c>
+      <c r="D483" s="0" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="0" t="n">
+        <v>483</v>
+      </c>
+      <c r="D484" s="0" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="0" t="n">
+        <v>484</v>
+      </c>
+      <c r="D485" s="0" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="0" t="n">
+        <v>485</v>
+      </c>
+      <c r="D486" s="0" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="0" t="n">
+        <v>486</v>
+      </c>
+      <c r="D487" s="0" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="0" t="n">
+        <v>487</v>
+      </c>
+      <c r="D488" s="0" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="0" t="n">
+        <v>488</v>
+      </c>
+      <c r="D489" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A490" s="0" t="n">
+        <v>489</v>
+      </c>
+      <c r="D490" s="0" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A491" s="0" t="n">
+        <v>490</v>
+      </c>
+      <c r="D491" s="0" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A492" s="0" t="n">
+        <v>491</v>
+      </c>
+      <c r="D492" s="0" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A493" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="D493" s="0" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A494" s="0" t="n">
+        <v>493</v>
+      </c>
+      <c r="D494" s="0" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A495" s="0" t="n">
+        <v>494</v>
+      </c>
+      <c r="D495" s="0" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="0" t="n">
+        <v>495</v>
+      </c>
+      <c r="D496" s="0" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A497" s="0" t="n">
+        <v>496</v>
+      </c>
+      <c r="D497" s="0" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A498" s="0" t="n">
+        <v>497</v>
+      </c>
+      <c r="D498" s="0" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A499" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="D499" s="0" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A500" s="0" t="n">
+        <v>499</v>
+      </c>
+      <c r="D500" s="0" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="D501" s="0" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="D502" s="0" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="0" t="n">
+        <v>502</v>
+      </c>
+      <c r="D503" s="0" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="0" t="n">
+        <v>503</v>
+      </c>
+      <c r="D504" s="0" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="0" t="n">
+        <v>504</v>
+      </c>
+      <c r="D505" s="0" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="0" t="n">
+        <v>505</v>
+      </c>
+      <c r="D506" s="0" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="0" t="n">
+        <v>506</v>
+      </c>
+      <c r="D507" s="0" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="0" t="n">
+        <v>507</v>
+      </c>
+      <c r="D508" s="0" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A509" s="0" t="n">
+        <v>508</v>
+      </c>
+      <c r="D509" s="0" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="0" t="n">
+        <v>509</v>
+      </c>
+      <c r="D510" s="0" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A511" s="0" t="n">
+        <v>510</v>
+      </c>
+      <c r="D511" s="0" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A512" s="0" t="n">
+        <v>511</v>
+      </c>
+      <c r="D512" s="0" t="s">
+        <v>1171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete overhaul of scripts
fixing bugs
enabling combined output of coordinates from GBIF and OBIS
improving warning messages
</commit_message>
<xml_diff>
--- a/Data/Input/AllLocations_DASCO.xlsx
+++ b/Data/Input/AllLocations_DASCO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="1172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="1188">
   <si>
     <t xml:space="preserve">locationID</t>
   </si>
@@ -2902,643 +2902,691 @@
     <t xml:space="preserve">Zimbabwe</t>
   </si>
   <si>
-    <t xml:space="preserve">Adriatic Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aegean Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agulhas Bank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alboran Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aleutian Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amsterdam-St Paul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amundsen/Bellingshausen Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andaman and Nicobar Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andaman Sea Coral Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angolan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antarctic Peninsula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arabian (Persian) Gulf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arafura Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Araucanian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arnhem Coast to Gulf of Carpenteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auckland Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azores Canaries Madeira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baffin Bay - Davis Strait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bahamian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baltic Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banda Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bassian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beaufort Sea - continental coast and shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beaufort-Amundsen-Viscount Melville-Queen Maud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bight of Sofala/Swamp Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bismarck Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonaparte Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bounty and Antipodes Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campbell Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cape Howe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cargados Carajos/Tromelin Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carolinian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celtic Seas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central and Southern Great Barrier Reef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Kuroshio Current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central New Zealand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Peru</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Somali Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channels and Fjords of Southern Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chatham Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chiapas-Nicaragua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chiloense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chukchi Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clipperton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cocos-Keeling/Christmas Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coral Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cortezian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delagoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East African Coral Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Antarctic Dronning Maud Land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Antarctic Enderby Land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Antarctic Wilkes Land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Caroline Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East China Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Greenland Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Siberian Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Bering Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Galapagos Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Philippines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exmouth to Broome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faroe Plateau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiji Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Floridian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gilbert/Ellis Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great Australian Bight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greater Antilles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guayaquil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guianan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Aden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Alaska</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Guinea Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Guinea Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Guinea South</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Guinea Upwelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Guinea West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Maine/Bay of Fundy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Oman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Papua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of St. Lawrence - Eastern Scotian Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Thailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gulf of Tonkin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halmahera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heard and Macdonald Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High Arctic Archipelago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Houtman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hudson Complex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Humboldtian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ionian Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamchatka Shelf and Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kara Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kermadec Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lancaster Sound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laptev Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leeuwin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lesser Sunda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Levantine Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Line Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lord Howe and Norfolk Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macquarie Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magdalena Transition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malacca Strait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malvinas/Falklands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manning-Hawkesbury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mariana Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marquesas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mascarene Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexican Tropical Pacific</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namaqua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicoya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ningaloo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North American Pacific Fijordland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North and East Barents Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North and East Iceland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North Greenland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North Patagonian Gulfs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northeast Sulawesi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northeastern Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northeastern Honshu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northeastern New Zealand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern and Central Red Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Bay of Bengal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern California</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Galapagos Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Grand Banks - Southern Labrador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Gulf of Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Labrador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Monsoon Current Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Norway and Finnmark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oregon, Washington, Vancouver Coast and Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oyashio Current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palawan/North Borneo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panama Bight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Papua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patagonian Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peter the First Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phoenix/Tokelau/Northern Cook Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puget Trough/Georgia Basin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rapa-Pitcairn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revillagigedos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de la Plata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio Grande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ross Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saharan Upwelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sahelian Upwelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samoa Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sao Pedro and Sao Paulo Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scotian Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sea of Japan/East Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sea of Okhotsk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shark Bay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snares Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Society Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solomon Archipelago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solomon Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South and West Iceland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Australian Gulfs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South European Atlantic Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Georgia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South India and Sri Lanka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Kuroshio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South New Zealand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Orkney Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Sandwich Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Shetland Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southeast Madagascar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southeast Papua New Guinea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southeastern Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern California Bight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Cook/Austral Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Grand Banks - South Newfoundland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Gulf of Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Norway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Red Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Vietnam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southwestern Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Helena and Ascension Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulawesi Sea/Makassar Strait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunda Shelf/Java Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Three Kings-North Cape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tonga Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torres Strait Northern Great Barrier Reef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trindade and Martin Vaz Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tristan Gough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuamotus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunisian Plateau/Gulf of Sidra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tweed-Moreton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uruguay-Buenos Aires Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virginian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weddell Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Caroline Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Greenland Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western and Northern Madagascar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Arabian Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Bassian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Galapagos Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Mediterranean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Sumatra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow Sea</t>
+    <t xml:space="preserve">Adriatic Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aegean Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agulhas Bank_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alboran Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleutian Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazonia_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amsterdam-St Paul_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amundsen/Bellingshausen Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andaman and Nicobar Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andaman Sea Coral Coast_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angolan_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctic Peninsula_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arabian (Persian) Gulf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arafura Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Araucanian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arnhem Coast to Gulf of Carpenteria_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auckland Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azores Canaries Madeira_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baffin Bay - Davis Strait_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bahamian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baltic Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banda Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bassian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaufort Sea - continental coast and shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaufort-Amundsen-Viscount Melville-Queen Maud_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bermuda_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bight of Sofala/Swamp Coast_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismarck Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonaparte Coast_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bounty and Antipodes Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouvet Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campbell Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Howe_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Verde_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cargados Carajos/Tromelin Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carolinian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celtic Seas_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central and Southern Great Barrier Reef_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Chile_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Kuroshio Current_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central New Zealand_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Peru_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Somali Coast_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chagos_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channels and Fjords of Southern Chile_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chatham Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiapas-Nicaragua_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiloense_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chukchi Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clipperton_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocos Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocos-Keeling/Christmas Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coral Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cortezian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crozet Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delagoa_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East African Coral Coast_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Antarctic Dronning Maud Land_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Antarctic Enderby Land_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Antarctic Wilkes Land_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Caroline Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East China Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Greenland Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Siberian Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easter Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Bering Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Brazil_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Caribbean_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Galapagos Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern India_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Philippines_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exmouth to Broome_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faroe Plateau_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fernando de Naronha and Atoll das Rocas_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiji Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floridian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gilbert/Ellis Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Australian Bight_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greater Antilles_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guayaquil_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guianan_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Aden_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Alaska_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea Central_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea South_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea Upwelling_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Guinea West_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Maine/Bay of Fundy_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Oman_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Papua_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of St. Lawrence - Eastern Scotian Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Thailand_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Tonkin_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halmahera_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heard and Macdonald Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Arctic Archipelago_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houtman_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hudson Complex_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humboldtian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ionian Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamchatka Shelf and Coast_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kara Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerguelen Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kermadec Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lancaster Sound_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptev Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leeuwin_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesser Sunda_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levantine Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lord Howe and Norfolk Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macquarie Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magdalena Transition_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malacca Strait_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maldives_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malvinas/Falklands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manning-Hawkesbury_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mariana Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquesas_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marshall Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mascarene Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexican Tropical Pacific_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namaqua_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namib_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natal_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Caledonia_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicoya_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ningaloo_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North American Pacific Fijordland_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North and East Barents Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North and East Iceland_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Greenland_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Patagonian Gulfs_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeast Sulawesi_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeastern Brazil_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeastern Honshu_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeastern New Zealand_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern and Central Red Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Bay of Bengal_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern California_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Galapagos Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Grand Banks - Southern Labrador_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Gulf of Mexico_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Labrador_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Monsoon Current Coast_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Norway and Finnmark_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ogasawara Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oregon, Washington, Vancouver Coast and Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oyashio Current_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palawan/North Borneo_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama Bight_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papua_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patagonian Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peter the First Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phoenix/Tokelau/Northern Cook Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puget Trough/Georgia Basin_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapa-Pitcairn_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revillagigedos_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio de la Plata_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rio Grande_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ross Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saharan Upwelling_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sahelian Upwelling_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samoa Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Pedro and Sao Paulo Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scotian Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea of Japan/East Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea of Okhotsk_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seychelles_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shark Bay_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snares Island_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Society Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solomon Archipelago_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solomon Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South and West Iceland_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Australian Gulfs_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South European Atlantic Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Georgia_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South India and Sri Lanka_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Kuroshio_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South New Zealand_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Orkney Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Sandwich Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Shetland Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeast Madagascar_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeast Papua New Guinea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeastern Brazil_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern California Bight_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Caribbean_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern China_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Cook/Austral Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Grand Banks - South Newfoundland_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Gulf of Mexico_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Java_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Norway_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Red Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Vietnam_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southwestern Caribbean_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Helena and Ascension Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulawesi Sea/Makassar Strait_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunda Shelf/Java Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three Kings-North Cape_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonga Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torres Strait Northern Great Barrier Reef_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trindade and Martin Vaz Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tristan Gough_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuamotus_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunisian Plateau/Gulf of Sidra_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tweed-Moreton_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uruguay-Buenos Aires Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanuatu_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weddell Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Caroline Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Greenland Shelf_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western and Northern Madagascar_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Arabian Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Bassian_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Caribbean_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Galapagos Islands_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western India_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Mediterranean_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Sumatra_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Sea_MEOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow Sea_MEOW</t>
   </si>
 </sst>
 </file>
@@ -3663,11 +3711,11 @@
   </sheetPr>
   <dimension ref="A1:K512"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A493" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D512" activeCellId="0" sqref="D512"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A282" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D284" activeCellId="0" sqref="D284"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.49"/>
@@ -12613,7 +12661,7 @@
         <v>308</v>
       </c>
       <c r="D309" s="0" t="s">
-        <v>115</v>
+        <v>984</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12621,7 +12669,7 @@
         <v>309</v>
       </c>
       <c r="D310" s="0" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12629,7 +12677,7 @@
         <v>310</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12637,7 +12685,7 @@
         <v>311</v>
       </c>
       <c r="D312" s="0" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12645,7 +12693,7 @@
         <v>312</v>
       </c>
       <c r="D313" s="0" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12653,7 +12701,7 @@
         <v>313</v>
       </c>
       <c r="D314" s="0" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12661,7 +12709,7 @@
         <v>314</v>
       </c>
       <c r="D315" s="0" t="s">
-        <v>144</v>
+        <v>990</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12669,7 +12717,7 @@
         <v>315</v>
       </c>
       <c r="D316" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12677,7 +12725,7 @@
         <v>316</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12685,7 +12733,7 @@
         <v>317</v>
       </c>
       <c r="D318" s="0" t="s">
-        <v>216</v>
+        <v>993</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12693,7 +12741,7 @@
         <v>318</v>
       </c>
       <c r="D319" s="0" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12701,7 +12749,7 @@
         <v>319</v>
       </c>
       <c r="D320" s="0" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12709,7 +12757,7 @@
         <v>320</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12717,7 +12765,7 @@
         <v>321</v>
       </c>
       <c r="D322" s="0" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12725,7 +12773,7 @@
         <v>322</v>
       </c>
       <c r="D323" s="0" t="s">
-        <v>995</v>
+        <v>998</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12733,7 +12781,7 @@
         <v>323</v>
       </c>
       <c r="D324" s="0" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12741,7 +12789,7 @@
         <v>324</v>
       </c>
       <c r="D325" s="0" t="s">
-        <v>997</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12749,7 +12797,7 @@
         <v>325</v>
       </c>
       <c r="D326" s="0" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12757,7 +12805,7 @@
         <v>326</v>
       </c>
       <c r="D327" s="0" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12765,7 +12813,7 @@
         <v>327</v>
       </c>
       <c r="D328" s="0" t="s">
-        <v>415</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12773,7 +12821,7 @@
         <v>328</v>
       </c>
       <c r="D329" s="0" t="s">
-        <v>1000</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12781,7 +12829,7 @@
         <v>329</v>
       </c>
       <c r="D330" s="0" t="s">
-        <v>1001</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12789,7 +12837,7 @@
         <v>330</v>
       </c>
       <c r="D331" s="0" t="s">
-        <v>1002</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12797,7 +12845,7 @@
         <v>331</v>
       </c>
       <c r="D332" s="0" t="s">
-        <v>1003</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12805,7 +12853,7 @@
         <v>332</v>
       </c>
       <c r="D333" s="0" t="s">
-        <v>1004</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12813,7 +12861,7 @@
         <v>333</v>
       </c>
       <c r="D334" s="0" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12821,7 +12869,7 @@
         <v>334</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>162</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12829,7 +12877,7 @@
         <v>335</v>
       </c>
       <c r="D336" s="0" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12837,7 +12885,7 @@
         <v>336</v>
       </c>
       <c r="D337" s="0" t="s">
-        <v>1007</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12845,7 +12893,7 @@
         <v>337</v>
       </c>
       <c r="D338" s="0" t="s">
-        <v>1008</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12853,7 +12901,7 @@
         <v>338</v>
       </c>
       <c r="D339" s="0" t="s">
-        <v>823</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12861,7 +12909,7 @@
         <v>339</v>
       </c>
       <c r="D340" s="0" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12869,7 +12917,7 @@
         <v>340</v>
       </c>
       <c r="D341" s="0" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12877,7 +12925,7 @@
         <v>341</v>
       </c>
       <c r="D342" s="0" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12885,7 +12933,7 @@
         <v>342</v>
       </c>
       <c r="D343" s="0" t="s">
-        <v>1012</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12893,7 +12941,7 @@
         <v>343</v>
       </c>
       <c r="D344" s="0" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12901,7 +12949,7 @@
         <v>344</v>
       </c>
       <c r="D345" s="0" t="s">
-        <v>1014</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12909,7 +12957,7 @@
         <v>345</v>
       </c>
       <c r="D346" s="0" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12917,7 +12965,7 @@
         <v>346</v>
       </c>
       <c r="D347" s="0" t="s">
-        <v>1016</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12925,7 +12973,7 @@
         <v>347</v>
       </c>
       <c r="D348" s="0" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12933,7 +12981,7 @@
         <v>348</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>196</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12941,7 +12989,7 @@
         <v>349</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>1018</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12949,7 +12997,7 @@
         <v>350</v>
       </c>
       <c r="D351" s="0" t="s">
-        <v>1019</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12957,7 +13005,7 @@
         <v>351</v>
       </c>
       <c r="D352" s="0" t="s">
-        <v>1020</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12965,7 +13013,7 @@
         <v>352</v>
       </c>
       <c r="D353" s="0" t="s">
-        <v>1021</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12973,7 +13021,7 @@
         <v>353</v>
       </c>
       <c r="D354" s="0" t="s">
-        <v>1022</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12981,7 +13029,7 @@
         <v>354</v>
       </c>
       <c r="D355" s="0" t="s">
-        <v>1023</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12989,7 +13037,7 @@
         <v>355</v>
       </c>
       <c r="D356" s="0" t="s">
-        <v>1024</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12997,7 +13045,7 @@
         <v>356</v>
       </c>
       <c r="D357" s="0" t="s">
-        <v>1025</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13005,7 +13053,7 @@
         <v>357</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>133</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13013,7 +13061,7 @@
         <v>358</v>
       </c>
       <c r="D359" s="0" t="s">
-        <v>1026</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13021,7 +13069,7 @@
         <v>359</v>
       </c>
       <c r="D360" s="0" t="s">
-        <v>1027</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13029,7 +13077,7 @@
         <v>360</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>1028</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13037,7 +13085,7 @@
         <v>361</v>
       </c>
       <c r="D362" s="0" t="s">
-        <v>1029</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13045,7 +13093,7 @@
         <v>362</v>
       </c>
       <c r="D363" s="0" t="s">
-        <v>1030</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13053,7 +13101,7 @@
         <v>363</v>
       </c>
       <c r="D364" s="0" t="s">
-        <v>1031</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13061,7 +13109,7 @@
         <v>364</v>
       </c>
       <c r="D365" s="0" t="s">
-        <v>1032</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13069,7 +13117,7 @@
         <v>365</v>
       </c>
       <c r="D366" s="0" t="s">
-        <v>1033</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13077,7 +13125,7 @@
         <v>366</v>
       </c>
       <c r="D367" s="0" t="s">
-        <v>1034</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13085,7 +13133,7 @@
         <v>367</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>1035</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13093,7 +13141,7 @@
         <v>368</v>
       </c>
       <c r="D369" s="0" t="s">
-        <v>1036</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13101,7 +13149,7 @@
         <v>369</v>
       </c>
       <c r="D370" s="0" t="s">
-        <v>1037</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13109,7 +13157,7 @@
         <v>370</v>
       </c>
       <c r="D371" s="0" t="s">
-        <v>1038</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13117,7 +13165,7 @@
         <v>371</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>1039</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13125,7 +13173,7 @@
         <v>372</v>
       </c>
       <c r="D373" s="0" t="s">
-        <v>1040</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13133,7 +13181,7 @@
         <v>373</v>
       </c>
       <c r="D374" s="0" t="s">
-        <v>1041</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13141,7 +13189,7 @@
         <v>374</v>
       </c>
       <c r="D375" s="0" t="s">
-        <v>1042</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13149,7 +13197,7 @@
         <v>375</v>
       </c>
       <c r="D376" s="0" t="s">
-        <v>1043</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13157,7 +13205,7 @@
         <v>376</v>
       </c>
       <c r="D377" s="0" t="s">
-        <v>1044</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13165,7 +13213,7 @@
         <v>377</v>
       </c>
       <c r="D378" s="0" t="s">
-        <v>1045</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13173,7 +13221,7 @@
         <v>378</v>
       </c>
       <c r="D379" s="0" t="s">
-        <v>1046</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13181,7 +13229,7 @@
         <v>379</v>
       </c>
       <c r="D380" s="0" t="s">
-        <v>895</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13189,7 +13237,7 @@
         <v>380</v>
       </c>
       <c r="D381" s="0" t="s">
-        <v>1047</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13197,7 +13245,7 @@
         <v>381</v>
       </c>
       <c r="D382" s="0" t="s">
-        <v>1048</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13205,7 +13253,7 @@
         <v>382</v>
       </c>
       <c r="D383" s="0" t="s">
-        <v>1049</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13213,7 +13261,7 @@
         <v>383</v>
       </c>
       <c r="D384" s="0" t="s">
-        <v>1050</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13221,7 +13269,7 @@
         <v>384</v>
       </c>
       <c r="D385" s="0" t="s">
-        <v>1051</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13229,7 +13277,7 @@
         <v>385</v>
       </c>
       <c r="D386" s="0" t="s">
-        <v>1052</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13237,7 +13285,7 @@
         <v>386</v>
       </c>
       <c r="D387" s="0" t="s">
-        <v>1053</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13245,7 +13293,7 @@
         <v>387</v>
       </c>
       <c r="D388" s="0" t="s">
-        <v>1054</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13253,7 +13301,7 @@
         <v>388</v>
       </c>
       <c r="D389" s="0" t="s">
-        <v>829</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13261,7 +13309,7 @@
         <v>389</v>
       </c>
       <c r="D390" s="0" t="s">
-        <v>1055</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13269,7 +13317,7 @@
         <v>390</v>
       </c>
       <c r="D391" s="0" t="s">
-        <v>1056</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13277,7 +13325,7 @@
         <v>391</v>
       </c>
       <c r="D392" s="0" t="s">
-        <v>1057</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13285,7 +13333,7 @@
         <v>392</v>
       </c>
       <c r="D393" s="0" t="s">
-        <v>1058</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13293,7 +13341,7 @@
         <v>393</v>
       </c>
       <c r="D394" s="0" t="s">
-        <v>1059</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13301,7 +13349,7 @@
         <v>394</v>
       </c>
       <c r="D395" s="0" t="s">
-        <v>1060</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13309,7 +13357,7 @@
         <v>395</v>
       </c>
       <c r="D396" s="0" t="s">
-        <v>1061</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13317,7 +13365,7 @@
         <v>396</v>
       </c>
       <c r="D397" s="0" t="s">
-        <v>1062</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13325,7 +13373,7 @@
         <v>397</v>
       </c>
       <c r="D398" s="0" t="s">
-        <v>1063</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13333,7 +13381,7 @@
         <v>398</v>
       </c>
       <c r="D399" s="0" t="s">
-        <v>1064</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13341,7 +13389,7 @@
         <v>399</v>
       </c>
       <c r="D400" s="0" t="s">
-        <v>1065</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13349,7 +13397,7 @@
         <v>400</v>
       </c>
       <c r="D401" s="0" t="s">
-        <v>602</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13357,7 +13405,7 @@
         <v>401</v>
       </c>
       <c r="D402" s="0" t="s">
-        <v>1066</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13365,7 +13413,7 @@
         <v>402</v>
       </c>
       <c r="D403" s="0" t="s">
-        <v>1067</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13373,7 +13421,7 @@
         <v>403</v>
       </c>
       <c r="D404" s="0" t="s">
-        <v>1068</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13381,7 +13429,7 @@
         <v>404</v>
       </c>
       <c r="D405" s="0" t="s">
-        <v>1069</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13389,7 +13437,7 @@
         <v>405</v>
       </c>
       <c r="D406" s="0" t="s">
-        <v>558</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13397,7 +13445,7 @@
         <v>406</v>
       </c>
       <c r="D407" s="0" t="s">
-        <v>1070</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13405,7 +13453,7 @@
         <v>407</v>
       </c>
       <c r="D408" s="0" t="s">
-        <v>1071</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13413,7 +13461,7 @@
         <v>408</v>
       </c>
       <c r="D409" s="0" t="s">
-        <v>1072</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13421,7 +13469,7 @@
         <v>409</v>
       </c>
       <c r="D410" s="0" t="s">
-        <v>1073</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13429,7 +13477,7 @@
         <v>410</v>
       </c>
       <c r="D411" s="0" t="s">
-        <v>1074</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13437,7 +13485,7 @@
         <v>411</v>
       </c>
       <c r="D412" s="0" t="s">
-        <v>623</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13445,7 +13493,7 @@
         <v>412</v>
       </c>
       <c r="D413" s="0" t="s">
-        <v>1075</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13453,7 +13501,7 @@
         <v>413</v>
       </c>
       <c r="D414" s="0" t="s">
-        <v>1076</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13461,7 +13509,7 @@
         <v>414</v>
       </c>
       <c r="D415" s="0" t="s">
-        <v>1077</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13469,7 +13517,7 @@
         <v>415</v>
       </c>
       <c r="D416" s="0" t="s">
-        <v>1078</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13477,7 +13525,7 @@
         <v>416</v>
       </c>
       <c r="D417" s="0" t="s">
-        <v>1079</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13485,7 +13533,7 @@
         <v>417</v>
       </c>
       <c r="D418" s="0" t="s">
-        <v>1080</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13493,7 +13541,7 @@
         <v>418</v>
       </c>
       <c r="D419" s="0" t="s">
-        <v>1081</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13501,7 +13549,7 @@
         <v>419</v>
       </c>
       <c r="D420" s="0" t="s">
-        <v>1082</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13509,7 +13557,7 @@
         <v>420</v>
       </c>
       <c r="D421" s="0" t="s">
-        <v>1083</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13517,7 +13565,7 @@
         <v>421</v>
       </c>
       <c r="D422" s="0" t="s">
-        <v>1084</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13525,7 +13573,7 @@
         <v>422</v>
       </c>
       <c r="D423" s="0" t="s">
-        <v>1085</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13533,7 +13581,7 @@
         <v>423</v>
       </c>
       <c r="D424" s="0" t="s">
-        <v>1086</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13541,7 +13589,7 @@
         <v>424</v>
       </c>
       <c r="D425" s="0" t="s">
-        <v>1087</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13549,7 +13597,7 @@
         <v>425</v>
       </c>
       <c r="D426" s="0" t="s">
-        <v>1088</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13557,7 +13605,7 @@
         <v>426</v>
       </c>
       <c r="D427" s="0" t="s">
-        <v>1089</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13565,7 +13613,7 @@
         <v>427</v>
       </c>
       <c r="D428" s="0" t="s">
-        <v>1090</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13573,7 +13621,7 @@
         <v>428</v>
       </c>
       <c r="D429" s="0" t="s">
-        <v>1091</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13581,7 +13629,7 @@
         <v>429</v>
       </c>
       <c r="D430" s="0" t="s">
-        <v>1092</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13589,7 +13637,7 @@
         <v>430</v>
       </c>
       <c r="D431" s="0" t="s">
-        <v>1093</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13597,7 +13645,7 @@
         <v>431</v>
       </c>
       <c r="D432" s="0" t="s">
-        <v>1094</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13605,7 +13653,7 @@
         <v>432</v>
       </c>
       <c r="D433" s="0" t="s">
-        <v>1095</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13613,7 +13661,7 @@
         <v>433</v>
       </c>
       <c r="D434" s="0" t="s">
-        <v>450</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13621,7 +13669,7 @@
         <v>434</v>
       </c>
       <c r="D435" s="0" t="s">
-        <v>1096</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13629,7 +13677,7 @@
         <v>435</v>
       </c>
       <c r="D436" s="0" t="s">
-        <v>1097</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13637,7 +13685,7 @@
         <v>436</v>
       </c>
       <c r="D437" s="0" t="s">
-        <v>1098</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13645,7 +13693,7 @@
         <v>437</v>
       </c>
       <c r="D438" s="0" t="s">
-        <v>1099</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13653,7 +13701,7 @@
         <v>438</v>
       </c>
       <c r="D439" s="0" t="s">
-        <v>1100</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13661,7 +13709,7 @@
         <v>439</v>
       </c>
       <c r="D440" s="0" t="s">
-        <v>1101</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13669,7 +13717,7 @@
         <v>440</v>
       </c>
       <c r="D441" s="0" t="s">
-        <v>1102</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13677,7 +13725,7 @@
         <v>441</v>
       </c>
       <c r="D442" s="0" t="s">
-        <v>1103</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13685,7 +13733,7 @@
         <v>442</v>
       </c>
       <c r="D443" s="0" t="s">
-        <v>1104</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13693,7 +13741,7 @@
         <v>443</v>
       </c>
       <c r="D444" s="0" t="s">
-        <v>1105</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13701,7 +13749,7 @@
         <v>444</v>
       </c>
       <c r="D445" s="0" t="s">
-        <v>1106</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13709,7 +13757,7 @@
         <v>445</v>
       </c>
       <c r="D446" s="0" t="s">
-        <v>1107</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13717,7 +13765,7 @@
         <v>446</v>
       </c>
       <c r="D447" s="0" t="s">
-        <v>1108</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13725,7 +13773,7 @@
         <v>447</v>
       </c>
       <c r="D448" s="0" t="s">
-        <v>1109</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13733,7 +13781,7 @@
         <v>448</v>
       </c>
       <c r="D449" s="0" t="s">
-        <v>1110</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13741,7 +13789,7 @@
         <v>449</v>
       </c>
       <c r="D450" s="0" t="s">
-        <v>1111</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13749,7 +13797,7 @@
         <v>450</v>
       </c>
       <c r="D451" s="0" t="s">
-        <v>1112</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13757,7 +13805,7 @@
         <v>451</v>
       </c>
       <c r="D452" s="0" t="s">
-        <v>1113</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13765,7 +13813,7 @@
         <v>452</v>
       </c>
       <c r="D453" s="0" t="s">
-        <v>1114</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13773,7 +13821,7 @@
         <v>453</v>
       </c>
       <c r="D454" s="0" t="s">
-        <v>1115</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13781,7 +13829,7 @@
         <v>454</v>
       </c>
       <c r="D455" s="0" t="s">
-        <v>1116</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13789,7 +13837,7 @@
         <v>455</v>
       </c>
       <c r="D456" s="0" t="s">
-        <v>747</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13797,7 +13845,7 @@
         <v>456</v>
       </c>
       <c r="D457" s="0" t="s">
-        <v>1117</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13805,7 +13853,7 @@
         <v>457</v>
       </c>
       <c r="D458" s="0" t="s">
-        <v>1118</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13813,7 +13861,7 @@
         <v>458</v>
       </c>
       <c r="D459" s="0" t="s">
-        <v>1119</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13821,7 +13869,7 @@
         <v>459</v>
       </c>
       <c r="D460" s="0" t="s">
-        <v>1120</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13829,7 +13877,7 @@
         <v>460</v>
       </c>
       <c r="D461" s="0" t="s">
-        <v>1121</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13837,7 +13885,7 @@
         <v>461</v>
       </c>
       <c r="D462" s="0" t="s">
-        <v>1122</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13845,7 +13893,7 @@
         <v>462</v>
       </c>
       <c r="D463" s="0" t="s">
-        <v>1123</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13853,7 +13901,7 @@
         <v>463</v>
       </c>
       <c r="D464" s="0" t="s">
-        <v>1124</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13861,7 +13909,7 @@
         <v>464</v>
       </c>
       <c r="D465" s="0" t="s">
-        <v>1125</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13869,7 +13917,7 @@
         <v>465</v>
       </c>
       <c r="D466" s="0" t="s">
-        <v>1126</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13877,7 +13925,7 @@
         <v>466</v>
       </c>
       <c r="D467" s="0" t="s">
-        <v>1127</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13885,7 +13933,7 @@
         <v>467</v>
       </c>
       <c r="D468" s="0" t="s">
-        <v>1128</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13893,7 +13941,7 @@
         <v>468</v>
       </c>
       <c r="D469" s="0" t="s">
-        <v>1129</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13901,7 +13949,7 @@
         <v>469</v>
       </c>
       <c r="D470" s="0" t="s">
-        <v>1130</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13909,7 +13957,7 @@
         <v>470</v>
       </c>
       <c r="D471" s="0" t="s">
-        <v>1131</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13917,7 +13965,7 @@
         <v>471</v>
       </c>
       <c r="D472" s="0" t="s">
-        <v>1132</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13925,7 +13973,7 @@
         <v>472</v>
       </c>
       <c r="D473" s="0" t="s">
-        <v>1133</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13933,7 +13981,7 @@
         <v>473</v>
       </c>
       <c r="D474" s="0" t="s">
-        <v>1134</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13941,7 +13989,7 @@
         <v>474</v>
       </c>
       <c r="D475" s="0" t="s">
-        <v>1135</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13949,7 +13997,7 @@
         <v>475</v>
       </c>
       <c r="D476" s="0" t="s">
-        <v>1136</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13957,7 +14005,7 @@
         <v>476</v>
       </c>
       <c r="D477" s="0" t="s">
-        <v>1137</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13965,7 +14013,7 @@
         <v>477</v>
       </c>
       <c r="D478" s="0" t="s">
-        <v>1138</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13973,7 +14021,7 @@
         <v>478</v>
       </c>
       <c r="D479" s="0" t="s">
-        <v>1139</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13981,7 +14029,7 @@
         <v>479</v>
       </c>
       <c r="D480" s="0" t="s">
-        <v>1140</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13989,7 +14037,7 @@
         <v>480</v>
       </c>
       <c r="D481" s="0" t="s">
-        <v>1141</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13997,7 +14045,7 @@
         <v>481</v>
       </c>
       <c r="D482" s="0" t="s">
-        <v>1142</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14005,7 +14053,7 @@
         <v>482</v>
       </c>
       <c r="D483" s="0" t="s">
-        <v>1143</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14013,7 +14061,7 @@
         <v>483</v>
       </c>
       <c r="D484" s="0" t="s">
-        <v>1144</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14021,7 +14069,7 @@
         <v>484</v>
       </c>
       <c r="D485" s="0" t="s">
-        <v>1145</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14029,7 +14077,7 @@
         <v>485</v>
       </c>
       <c r="D486" s="0" t="s">
-        <v>1146</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14037,7 +14085,7 @@
         <v>486</v>
       </c>
       <c r="D487" s="0" t="s">
-        <v>1147</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14045,7 +14093,7 @@
         <v>487</v>
       </c>
       <c r="D488" s="0" t="s">
-        <v>1148</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14053,7 +14101,7 @@
         <v>488</v>
       </c>
       <c r="D489" s="0" t="s">
-        <v>1149</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14061,7 +14109,7 @@
         <v>489</v>
       </c>
       <c r="D490" s="0" t="s">
-        <v>1150</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14069,7 +14117,7 @@
         <v>490</v>
       </c>
       <c r="D491" s="0" t="s">
-        <v>1151</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14077,7 +14125,7 @@
         <v>491</v>
       </c>
       <c r="D492" s="0" t="s">
-        <v>1152</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14085,7 +14133,7 @@
         <v>492</v>
       </c>
       <c r="D493" s="0" t="s">
-        <v>1153</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14093,7 +14141,7 @@
         <v>493</v>
       </c>
       <c r="D494" s="0" t="s">
-        <v>1154</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14101,7 +14149,7 @@
         <v>494</v>
       </c>
       <c r="D495" s="0" t="s">
-        <v>1155</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14109,7 +14157,7 @@
         <v>495</v>
       </c>
       <c r="D496" s="0" t="s">
-        <v>1156</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14117,7 +14165,7 @@
         <v>496</v>
       </c>
       <c r="D497" s="0" t="s">
-        <v>1157</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14125,7 +14173,7 @@
         <v>497</v>
       </c>
       <c r="D498" s="0" t="s">
-        <v>934</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14133,7 +14181,7 @@
         <v>498</v>
       </c>
       <c r="D499" s="0" t="s">
-        <v>1158</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14141,7 +14189,7 @@
         <v>499</v>
       </c>
       <c r="D500" s="0" t="s">
-        <v>1159</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14149,7 +14197,7 @@
         <v>500</v>
       </c>
       <c r="D501" s="0" t="s">
-        <v>1160</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14157,7 +14205,7 @@
         <v>501</v>
       </c>
       <c r="D502" s="0" t="s">
-        <v>1161</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14165,7 +14213,7 @@
         <v>502</v>
       </c>
       <c r="D503" s="0" t="s">
-        <v>1162</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14173,7 +14221,7 @@
         <v>503</v>
       </c>
       <c r="D504" s="0" t="s">
-        <v>1163</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14181,7 +14229,7 @@
         <v>504</v>
       </c>
       <c r="D505" s="0" t="s">
-        <v>1164</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14189,7 +14237,7 @@
         <v>505</v>
       </c>
       <c r="D506" s="0" t="s">
-        <v>1165</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14197,7 +14245,7 @@
         <v>506</v>
       </c>
       <c r="D507" s="0" t="s">
-        <v>1166</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14205,7 +14253,7 @@
         <v>507</v>
       </c>
       <c r="D508" s="0" t="s">
-        <v>1167</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14213,7 +14261,7 @@
         <v>508</v>
       </c>
       <c r="D509" s="0" t="s">
-        <v>1168</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14221,7 +14269,7 @@
         <v>509</v>
       </c>
       <c r="D510" s="0" t="s">
-        <v>1169</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14229,7 +14277,7 @@
         <v>510</v>
       </c>
       <c r="D511" s="0" t="s">
-        <v>1170</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14237,7 +14285,7 @@
         <v>511</v>
       </c>
       <c r="D512" s="0" t="s">
-        <v>1171</v>
+        <v>1187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>